<commit_message>
Adding equation for bottle with no angle
</commit_message>
<xml_diff>
--- a/distance_in_fct_height_ratio.xlsx
+++ b/distance_in_fct_height_ratio.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\antho\Documents\GitHub\Visual_recognition\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E897CE43-3385-4AC4-BEAB-9432EDF400E9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40EA6500-421A-485B-BFDF-09FC191F3957}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" xr2:uid="{728A45A0-F77A-4BD6-AD45-D6A58E7F6F94}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>height</t>
   </si>
@@ -40,15 +40,52 @@
   <si>
     <t>distance</t>
   </si>
+  <si>
+    <t>Equation</t>
+  </si>
+  <si>
+    <r>
+      <t>y = 18025x</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="9"/>
+        <color rgb="FF595959"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>-1.038</t>
+    </r>
+  </si>
+  <si>
+    <t>mean ratio</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF595959"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <vertAlign val="superscript"/>
+      <sz val="9"/>
+      <color rgb="FF595959"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -74,8 +111,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -91,6 +131,1013 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>distance</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="power"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-1.9110892388451442E-2"/>
+                  <c:y val="-0.24197324292796735"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$2:$A$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>469</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>294</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>202</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>154</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>119</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>97</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>76</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>66</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>59</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>51</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$2:$C$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>130</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>230</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>260</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>300</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-EE32-4019-8FAC-A858897900FD}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="433055248"/>
+        <c:axId val="433057544"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="433055248"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="433057544"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="433057544"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="433055248"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>312420</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>160020</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>7620</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>160020</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BF1F100A-F026-4D7F-8B5E-9C94934A04C2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -390,15 +1437,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBEE5061-762F-4FCE-B7DE-8B138EE3F1C3}">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="4" max="4" width="13.109375" customWidth="1"/>
+    <col min="5" max="5" width="9.88671875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -408,8 +1459,14 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>469</v>
       </c>
@@ -420,7 +1477,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>294</v>
       </c>
@@ -431,7 +1488,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>202</v>
       </c>
@@ -442,7 +1499,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>154</v>
       </c>
@@ -453,7 +1510,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>119</v>
       </c>
@@ -464,7 +1521,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>97</v>
       </c>
@@ -475,7 +1532,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>76</v>
       </c>
@@ -486,7 +1543,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>66</v>
       </c>
@@ -497,7 +1554,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>59</v>
       </c>
@@ -508,7 +1565,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>51</v>
       </c>
@@ -517,9 +1574,17 @@
       </c>
       <c r="C11">
         <v>300</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E11">
+        <f>AVERAGE(B2:B11)</f>
+        <v>3.1840000000000002</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Adding Adding equation for no angle bottle
</commit_message>
<xml_diff>
--- a/distance_in_fct_height_ratio.xlsx
+++ b/distance_in_fct_height_ratio.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\antho\Documents\GitHub\Visual_recognition\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40EA6500-421A-485B-BFDF-09FC191F3957}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71165586-9A32-4558-81F4-C17084867262}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" xr2:uid="{728A45A0-F77A-4BD6-AD45-D6A58E7F6F94}"/>
   </bookViews>
@@ -237,8 +237,8 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-1.9110892388451442E-2"/>
-                  <c:y val="-0.24197324292796735"/>
+                  <c:x val="-0.11911089238845145"/>
+                  <c:y val="-0.32993620589093031"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -352,7 +352,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-EE32-4019-8FAC-A858897900FD}"/>
+              <c16:uniqueId val="{00000000-616E-408C-BA16-CEABCEFC180F}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -364,11 +364,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="433055248"/>
-        <c:axId val="433057544"/>
+        <c:axId val="442884480"/>
+        <c:axId val="442883496"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="433055248"/>
+        <c:axId val="442884480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -425,12 +425,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="433057544"/>
+        <c:crossAx val="442883496"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="433057544"/>
+        <c:axId val="442883496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -487,7 +487,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="433055248"/>
+        <c:crossAx val="442884480"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1103,23 +1103,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>312420</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>160020</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>106680</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>34290</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>7620</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>160020</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>34290</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2">
+        <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BF1F100A-F026-4D7F-8B5E-9C94934A04C2}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{22CF0BC4-C769-4AC1-87E8-5AA7A72BC6C0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1440,11 +1440,12 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.109375" customWidth="1"/>
     <col min="5" max="5" width="9.88671875" customWidth="1"/>
   </cols>

</xml_diff>

<commit_message>
Find distance even if bottle has angle
</commit_message>
<xml_diff>
--- a/distance_in_fct_height_ratio.xlsx
+++ b/distance_in_fct_height_ratio.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\antho\Documents\GitHub\Visual_recognition\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71165586-9A32-4558-81F4-C17084867262}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E62B5CA-5965-41D9-8DAB-5412D32921F0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" xr2:uid="{728A45A0-F77A-4BD6-AD45-D6A58E7F6F94}"/>
   </bookViews>
@@ -241,6 +241,36 @@
                   <c:y val="-0.32993620589093031"/>
                 </c:manualLayout>
               </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:pPr>
+                      <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                        <a:solidFill>
+                          <a:schemeClr val="tx1">
+                            <a:lumMod val="65000"/>
+                            <a:lumOff val="35000"/>
+                          </a:schemeClr>
+                        </a:solidFill>
+                        <a:latin typeface="+mn-lt"/>
+                        <a:ea typeface="+mn-ea"/>
+                        <a:cs typeface="+mn-cs"/>
+                      </a:defRPr>
+                    </a:pPr>
+                    <a:r>
+                      <a:rPr lang="en-GB" sz="2400" baseline="0"/>
+                      <a:t>y = 18025x</a:t>
+                    </a:r>
+                    <a:r>
+                      <a:rPr lang="en-GB" sz="2400" baseline="30000"/>
+                      <a:t>-1.038</a:t>
+                    </a:r>
+                    <a:endParaRPr lang="en-GB" sz="2400"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -543,7 +573,446 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="power"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-9.9647856517935257E-3"/>
+                  <c:y val="-0.38738699329250509"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:pPr>
+                      <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                        <a:solidFill>
+                          <a:schemeClr val="tx1">
+                            <a:lumMod val="65000"/>
+                            <a:lumOff val="35000"/>
+                          </a:schemeClr>
+                        </a:solidFill>
+                        <a:latin typeface="+mn-lt"/>
+                        <a:ea typeface="+mn-ea"/>
+                        <a:cs typeface="+mn-cs"/>
+                      </a:defRPr>
+                    </a:pPr>
+                    <a:r>
+                      <a:rPr lang="en-US" sz="2800" baseline="0"/>
+                      <a:t>y = 5766.7x</a:t>
+                    </a:r>
+                    <a:r>
+                      <a:rPr lang="en-US" sz="2800" baseline="30000"/>
+                      <a:t>-0.872</a:t>
+                    </a:r>
+                    <a:endParaRPr lang="en-US" sz="2800"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$13:$A$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>320</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>146</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>88</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>51</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>35</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$13:$C$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>190</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>270</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-2583-4782-BBE7-64DEE7FC7340}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="429917056"/>
+        <c:axId val="429915416"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="429917056"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="429915416"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="429915416"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="429917056"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -1099,20 +1568,536 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>106680</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>34290</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>87630</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>342900</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>34290</xdr:rowOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>87630</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1132,6 +2117,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>22860</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>22860</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{651E289F-61C1-4A31-B186-0BABC5D4AC33}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1437,10 +2458,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBEE5061-762F-4FCE-B7DE-8B138EE3F1C3}">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1584,6 +2605,64 @@
         <v>3.1840000000000002</v>
       </c>
     </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>320</v>
+      </c>
+      <c r="B13">
+        <v>2.64</v>
+      </c>
+      <c r="C13">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>146</v>
+      </c>
+      <c r="B14">
+        <v>2.39</v>
+      </c>
+      <c r="C14">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>88</v>
+      </c>
+      <c r="B15">
+        <v>2.04</v>
+      </c>
+      <c r="C15">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>51</v>
+      </c>
+      <c r="B16">
+        <v>1.75</v>
+      </c>
+      <c r="C16">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>35</v>
+      </c>
+      <c r="B17">
+        <v>1.75</v>
+      </c>
+      <c r="C17">
+        <v>270</v>
+      </c>
+      <c r="E17">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>